<commit_message>
Reorder test files: OBP, SLG
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fall 2015 09.16" sheetId="4" r:id="rId1"/>
@@ -119,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -136,6 +136,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -171,8 +183,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -184,7 +204,15 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -516,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -578,10 +606,10 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>15</v>
@@ -631,15 +659,15 @@
         <v>0.75</v>
       </c>
       <c r="O2" s="6">
-        <f t="shared" ref="O2:O5" si="1">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
+        <f>IF(B2,(E2+J2)/(C2+J2+L2),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P2" s="6">
+        <f t="shared" ref="P2:P5" si="1">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
         <v>1.5</v>
       </c>
-      <c r="P2" s="6">
-        <f t="shared" ref="P2:P6" si="2">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
-        <v>0.8</v>
-      </c>
       <c r="Q2" s="6">
-        <f t="shared" ref="Q2:Q6" si="3">IF(O2,O2+P2,)</f>
+        <f>IF(P2,P2+O2,)</f>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -686,15 +714,15 @@
         <v>0.8</v>
       </c>
       <c r="O3" s="6">
+        <f>IF(B3,(E3+J3)/(C3+J3+L3),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P3" s="6">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="P3" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q3" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P3,P3+O3,)</f>
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -741,15 +769,15 @@
         <v>0.75</v>
       </c>
       <c r="O4" s="6">
+        <f>IF(B4,(E4+J4)/(C4+J4+L4),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P4" s="6">
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q4" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P4,P4+O4,)</f>
         <v>2.5499999999999998</v>
       </c>
     </row>
@@ -796,15 +824,15 @@
         <v>0.8</v>
       </c>
       <c r="O5" s="6">
+        <f>IF(B5,(E5+J5)/(C5+J5+L5),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P5" s="6">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
-      <c r="P5" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q5" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P5,P5+O5,)</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -813,47 +841,47 @@
         <v>28</v>
       </c>
       <c r="B6" s="2">
-        <f>SUM(B2:B5)</f>
+        <f t="shared" ref="B6:L6" si="2">SUM(B2:B5)</f>
         <v>20</v>
       </c>
       <c r="C6" s="2">
-        <f>SUM(C2:C5)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D6" s="2">
-        <f>SUM(D2:D5)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E6" s="2">
-        <f>SUM(E2:E5)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="F6" s="2">
-        <f>SUM(F2:F5)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="G6" s="2">
-        <f>SUM(G2:G5)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H6" s="2">
-        <f>SUM(H2:H5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f>SUM(I2:I5)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="J6" s="2">
-        <f>SUM(J2:J5)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K6" s="2">
-        <f>SUM(K2:K5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <f>SUM(L2:L5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M6" s="5"/>
@@ -862,15 +890,15 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="O6" s="7">
+        <f>IF(B6,(E6+J6)/(C6+J6+L6),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P6" s="7">
         <f>((E6-F6-G6-H6)+(2*F6)+(3*G6)+(4*H6))/C6</f>
         <v>1.5555555555555556</v>
       </c>
-      <c r="P6" s="7">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q6" s="7">
-        <f t="shared" si="3"/>
+        <f>IF(P6,P6+O6,)</f>
         <v>2.3555555555555556</v>
       </c>
     </row>
@@ -882,6 +910,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -895,7 +924,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -956,10 +985,10 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>15</v>
@@ -1009,15 +1038,15 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="O2" s="6">
-        <f t="shared" ref="O2:O5" si="1">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
+        <f>IF(B2,(E2+J2)/(C2+J2+L2),)</f>
+        <v>0.75</v>
+      </c>
+      <c r="P2" s="6">
+        <f t="shared" ref="P2:P5" si="1">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="P2" s="6">
-        <f t="shared" ref="P2:P6" si="2">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
-        <v>0.75</v>
-      </c>
       <c r="Q2" s="6">
-        <f t="shared" ref="Q2:Q6" si="3">IF(O2,O2+P2,)</f>
+        <f>IF(P2,P2+O2,)</f>
         <v>1.4166666666666665</v>
       </c>
     </row>
@@ -1064,15 +1093,15 @@
         <v>0.8</v>
       </c>
       <c r="O3" s="6">
+        <f>IF(B3,(E3+J3)/(C3+J3+L3),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P3" s="6">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="P3" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q3" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P3,P3+O3,)</f>
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -1119,15 +1148,15 @@
         <v>0.75</v>
       </c>
       <c r="O4" s="6">
+        <f>IF(B4,(E4+J4)/(C4+J4+L4),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P4" s="6">
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q4" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P4,P4+O4,)</f>
         <v>2.5499999999999998</v>
       </c>
     </row>
@@ -1174,15 +1203,15 @@
         <v>0.8</v>
       </c>
       <c r="O5" s="6">
+        <f>IF(B5,(E5+J5)/(C5+J5+L5),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P5" s="6">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
-      <c r="P5" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q5" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P5,P5+O5,)</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -1191,47 +1220,47 @@
         <v>28</v>
       </c>
       <c r="B6" s="2">
-        <f>SUM(B2:B5)</f>
+        <f t="shared" ref="B6:L6" si="2">SUM(B2:B5)</f>
         <v>19</v>
       </c>
       <c r="C6" s="2">
-        <f>SUM(C2:C5)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="D6" s="2">
-        <f>SUM(D2:D5)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E6" s="2">
-        <f>SUM(E2:E5)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="F6" s="2">
-        <f>SUM(F2:F5)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G6" s="2">
-        <f>SUM(G2:G5)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H6" s="2">
-        <f>SUM(H2:H5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f>SUM(I2:I5)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J6" s="2">
-        <f>SUM(J2:J5)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K6" s="2">
-        <f>SUM(K2:K5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <f>SUM(L2:L5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M6" s="5"/>
@@ -1240,15 +1269,15 @@
         <v>0.76470588235294112</v>
       </c>
       <c r="O6" s="7">
+        <f>IF(B6,(E6+J6)/(C6+J6+L6),)</f>
+        <v>0.78947368421052633</v>
+      </c>
+      <c r="P6" s="7">
         <f>((E6-F6-G6-H6)+(2*F6)+(3*G6)+(4*H6))/C6</f>
         <v>1.411764705882353</v>
       </c>
-      <c r="P6" s="7">
-        <f t="shared" si="2"/>
-        <v>0.78947368421052633</v>
-      </c>
       <c r="Q6" s="7">
-        <f t="shared" si="3"/>
+        <f>IF(P6,P6+O6,)</f>
         <v>2.2012383900928794</v>
       </c>
     </row>
@@ -1260,6 +1289,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1273,7 +1303,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1334,10 +1364,10 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>15</v>
@@ -1387,15 +1417,15 @@
         <v>0.75</v>
       </c>
       <c r="O2" s="6">
-        <f t="shared" ref="O2:O5" si="1">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
+        <f>IF(B2,(E2+J2)/(C2+J2+L2),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P2" s="6">
+        <f t="shared" ref="P2:P5" si="1">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
         <v>1.5</v>
       </c>
-      <c r="P2" s="6">
-        <f t="shared" ref="P2:P6" si="2">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
-        <v>0.8</v>
-      </c>
       <c r="Q2" s="6">
-        <f t="shared" ref="Q2:Q6" si="3">IF(O2,O2+P2,)</f>
+        <f>IF(P2,P2+O2,)</f>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -1442,15 +1472,15 @@
         <v>0.8</v>
       </c>
       <c r="O3" s="6">
+        <f>IF(B3,(E3+J3)/(C3+J3+L3),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P3" s="6">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="P3" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q3" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P3,P3+O3,)</f>
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -1497,15 +1527,15 @@
         <v>0.75</v>
       </c>
       <c r="O4" s="6">
+        <f>IF(B4,(E4+J4)/(C4+J4+L4),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P4" s="6">
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q4" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P4,P4+O4,)</f>
         <v>2.5499999999999998</v>
       </c>
     </row>
@@ -1552,15 +1582,15 @@
         <v>0.8</v>
       </c>
       <c r="O5" s="6">
+        <f>IF(B5,(E5+J5)/(C5+J5+L5),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P5" s="6">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
-      <c r="P5" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q5" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P5,P5+O5,)</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -1569,47 +1599,47 @@
         <v>28</v>
       </c>
       <c r="B6" s="2">
-        <f>SUM(B2:B5)</f>
+        <f t="shared" ref="B6:L6" si="2">SUM(B2:B5)</f>
         <v>20</v>
       </c>
       <c r="C6" s="2">
-        <f>SUM(C2:C5)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D6" s="2">
-        <f>SUM(D2:D5)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E6" s="2">
-        <f>SUM(E2:E5)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="F6" s="2">
-        <f>SUM(F2:F5)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="G6" s="2">
-        <f>SUM(G2:G5)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H6" s="2">
-        <f>SUM(H2:H5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f>SUM(I2:I5)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J6" s="2">
-        <f>SUM(J2:J5)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K6" s="2">
-        <f>SUM(K2:K5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <f>SUM(L2:L5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M6" s="5"/>
@@ -1618,15 +1648,15 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="O6" s="7">
+        <f>IF(B6,(E6+J6)/(C6+J6+L6),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P6" s="7">
         <f>((E6-F6-G6-H6)+(2*F6)+(3*G6)+(4*H6))/C6</f>
         <v>1.5555555555555556</v>
       </c>
-      <c r="P6" s="7">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q6" s="7">
-        <f t="shared" si="3"/>
+        <f>IF(P6,P6+O6,)</f>
         <v>2.3555555555555556</v>
       </c>
     </row>
@@ -1638,6 +1668,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1650,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1712,10 +1743,10 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>15</v>
@@ -1765,15 +1796,15 @@
         <v>0.75</v>
       </c>
       <c r="O2" s="6">
-        <f t="shared" ref="O2:O5" si="1">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
+        <f>IF(B2,(E2+J2)/(C2+J2+L2),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P2" s="6">
+        <f t="shared" ref="P2:P5" si="1">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
         <v>1.5</v>
       </c>
-      <c r="P2" s="6">
-        <f t="shared" ref="P2:P6" si="2">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
-        <v>0.8</v>
-      </c>
       <c r="Q2" s="6">
-        <f t="shared" ref="Q2:Q6" si="3">IF(O2,O2+P2,)</f>
+        <f>IF(P2,P2+O2,)</f>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -1820,15 +1851,15 @@
         <v>0.8</v>
       </c>
       <c r="O3" s="6">
+        <f>IF(B3,(E3+J3)/(C3+J3+L3),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P3" s="6">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="P3" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q3" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P3,P3+O3,)</f>
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -1875,15 +1906,15 @@
         <v>0.75</v>
       </c>
       <c r="O4" s="6">
+        <f>IF(B4,(E4+J4)/(C4+J4+L4),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P4" s="6">
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q4" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P4,P4+O4,)</f>
         <v>2.5499999999999998</v>
       </c>
     </row>
@@ -1930,15 +1961,15 @@
         <v>0.8</v>
       </c>
       <c r="O5" s="6">
+        <f>IF(B5,(E5+J5)/(C5+J5+L5),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P5" s="6">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
-      <c r="P5" s="6">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q5" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(P5,P5+O5,)</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -1947,47 +1978,47 @@
         <v>28</v>
       </c>
       <c r="B6" s="2">
-        <f>SUM(B2:B5)</f>
+        <f t="shared" ref="B6:L6" si="2">SUM(B2:B5)</f>
         <v>20</v>
       </c>
       <c r="C6" s="2">
-        <f>SUM(C2:C5)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D6" s="2">
-        <f>SUM(D2:D5)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E6" s="2">
-        <f>SUM(E2:E5)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="F6" s="2">
-        <f>SUM(F2:F5)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="G6" s="2">
-        <f>SUM(G2:G5)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H6" s="2">
-        <f>SUM(H2:H5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f>SUM(I2:I5)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="J6" s="2">
-        <f>SUM(J2:J5)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K6" s="2">
-        <f>SUM(K2:K5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <f>SUM(L2:L5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M6" s="5"/>
@@ -1996,15 +2027,15 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="O6" s="7">
+        <f>IF(B6,(E6+J6)/(C6+J6+L6),)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P6" s="7">
         <f>((E6-F6-G6-H6)+(2*F6)+(3*G6)+(4*H6))/C6</f>
         <v>1.5555555555555556</v>
       </c>
-      <c r="P6" s="7">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
       <c r="Q6" s="7">
-        <f t="shared" si="3"/>
+        <f>IF(P6,P6+O6,)</f>
         <v>2.3555555555555556</v>
       </c>
     </row>
@@ -2016,6 +2047,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>